<commit_message>
gateway_extraction_confidence_per_type analysis on TEST_DOCS
</commit_message>
<xml_diff>
--- a/data/paper_stats/activity_relation/gateway_extraction/rc=goldstandard_vote_comparison.xlsx
+++ b/data/paper_stats/activity_relation/gateway_extraction/rc=goldstandard_vote_comparison.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janek\Development\Git\master-thesis\data\paper_stats\activity_relation\gateway_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E5E612-E86A-40C5-87A7-C21C24B1420D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799A9A91-0A96-4FA1-B729-744063324374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18585" yWindow="5760" windowWidth="17280" windowHeight="8970" xr2:uid="{D7FB8BA9-69F7-4C91-B2FE-97FA3C39EEFF}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D7FB8BA9-69F7-4C91-B2FE-97FA3C39EEFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Docs" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +38,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={E32E490C-1C26-497B-A420-D3B54811EFD8}</author>
+    <author>tc={CDAED81C-4E63-4622-A8FE-8FEB977ADE0B}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E32E490C-1C26-497B-A420-D3B54811EFD8}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{CDAED81C-4E63-4622-A8FE-8FEB977ADE0B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Label</t>
   </si>
@@ -90,13 +90,22 @@
   </si>
   <si>
     <t>confidence score</t>
+  </si>
+  <si>
+    <t>Docs</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Test Docs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,10 +119,24 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -228,11 +251,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -258,8 +312,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,81 +674,90 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F1" dT="2023-02-03T06:32:28.71" personId="{A53B3561-AFB1-4B9D-A9D8-C9F546232D48}" id="{E32E490C-1C26-497B-A420-D3B54811EFD8}">
+  <threadedComment ref="G1" dT="2023-02-03T06:32:28.71" personId="{A53B3561-AFB1-4B9D-A9D8-C9F546232D48}" id="{CDAED81C-4E63-4622-A8FE-8FEB977ADE0B}">
     <text>Computed with gateway_extraction_confidence_per_type</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522072C6-FE57-4AB4-A7A2-F368D0683D27}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0907E7E4-10FA-402E-9A73-20E0112AE3DC}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0.86</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.86</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.86</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.94</v>
-      </c>
-      <c r="G2" s="6">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.91</v>
+      </c>
+      <c r="H2" s="6">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.75</v>
       </c>
       <c r="D3" s="7">
         <v>0.75</v>
@@ -666,101 +768,273 @@
       <c r="F3" s="7">
         <v>0.75</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.85</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.85</v>
-      </c>
-      <c r="F4" s="8">
-        <f>(F2*G2+F3*G3) /(G2+G3)</f>
-        <v>0.91945945945945939</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="D4" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="G4" s="11">
+        <f>(G2*H2+G3*H3) /(H2+H3)</f>
+        <v>0.89270270270270269</v>
+      </c>
+      <c r="H4" s="8">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.91</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.98</v>
+      </c>
+      <c r="H5" s="7">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="18">
         <v>0.62</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="18">
         <v>0.62</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="18">
         <v>0.62</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
-        <v>0.81</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.81</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.81</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="D7" s="18">
+        <v>0.87</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.88</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.87</v>
+      </c>
+      <c r="G7" s="13">
+        <f>(G5*H5+G6*H6) /(H5+H6)</f>
+        <v>0.98216216216216201</v>
+      </c>
+      <c r="H7" s="7">
         <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>